<commit_message>
Write to Excel, must use two files.
</commit_message>
<xml_diff>
--- a/app/data/Input.xlsx
+++ b/app/data/Input.xlsx
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -390,7 +390,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ADX</t>
         </is>
       </c>
     </row>
@@ -405,7 +405,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ABT</t>
+          <t>AMH</t>
         </is>
       </c>
     </row>
@@ -420,7 +420,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ADX</t>
+          <t>APO</t>
         </is>
       </c>
     </row>
@@ -435,7 +435,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AHH</t>
+          <t>BC</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AMAT</t>
+          <t>BDN</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AMH</t>
+          <t>BHF</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>APD</t>
+          <t>CDNS</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>APO</t>
+          <t>CG</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ASPU</t>
+          <t>CLW</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ATKR</t>
+          <t>CTXS</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>BGCP</t>
+          <t>DHI</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BHE</t>
+          <t>DOOR</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BMCH</t>
+          <t>EGP</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CAH</t>
+          <t>ELAN</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CDNS</t>
+          <t>EWBC</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CG</t>
+          <t>EXC</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CIT</t>
+          <t>EXLS</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>COF</t>
+          <t>FE</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CPRT</t>
+          <t>FR</t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CSWC</t>
+          <t>GRBK</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CTXS</t>
+          <t>HE</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>DGX</t>
+          <t>HR</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>DHI</t>
+          <t>IBP</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>DOOR</t>
+          <t>INTC</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ELAN</t>
+          <t>ITGR</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>EVR</t>
+          <t>IVR</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>EXC</t>
+          <t>JBGS</t>
         </is>
       </c>
     </row>
@@ -795,7 +795,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>EXLS</t>
+          <t>JKHY</t>
         </is>
       </c>
     </row>
@@ -810,7 +810,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>EXP</t>
+          <t>KBH</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>FE</t>
+          <t>KO</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FISV</t>
+          <t>LEN</t>
         </is>
       </c>
     </row>
@@ -855,7 +855,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>GOOG</t>
+          <t>LMT</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>GOOGL</t>
+          <t>LNT</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>GPN</t>
+          <t>LQDA</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>GRBK</t>
+          <t>MDU</t>
         </is>
       </c>
     </row>
@@ -915,7 +915,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>HE</t>
+          <t>MRCC</t>
         </is>
       </c>
     </row>
@@ -930,7 +930,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>HUBB</t>
+          <t>MU</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>IBP</t>
+          <t>MYE</t>
         </is>
       </c>
     </row>
@@ -960,7 +960,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ICAD</t>
+          <t>NDSN</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>IIIV</t>
+          <t>NOVA</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>NX</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ITGR</t>
+          <t>OPI</t>
         </is>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>IVR</t>
+          <t>ORC</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>JKHY</t>
+          <t>PDM</t>
         </is>
       </c>
     </row>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>KBH</t>
+          <t>PEG</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>KLAC</t>
+          <t>PEP</t>
         </is>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>PGRE</t>
         </is>
       </c>
     </row>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>LAMR</t>
+          <t>PHR</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>LEN</t>
+          <t>PLXS</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>LLY</t>
+          <t>PRIM</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>LNT</t>
+          <t>PTC</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>LOW</t>
+          <t>RMBS</t>
         </is>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>LQDA</t>
+          <t>SLG</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LRCX</t>
+          <t>SO</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MCO</t>
+          <t>SRE</t>
         </is>
       </c>
     </row>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MDT</t>
+          <t>SSD</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MRCC</t>
+          <t>STWD</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MU</t>
+          <t>TWO</t>
         </is>
       </c>
     </row>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MWA</t>
+          <t>UMH</t>
         </is>
       </c>
     </row>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MXL</t>
+          <t>UNP</t>
         </is>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>NDSN</t>
+          <t>VNO</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>NOVA</t>
+          <t>WDC</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>WRB</t>
         </is>
       </c>
     </row>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>NYMT</t>
+          <t>XAN</t>
         </is>
       </c>
     </row>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>OESX</t>
+          <t>YMAB</t>
         </is>
       </c>
     </row>
@@ -1360,12 +1360,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>OPI</t>
+          <t>AAWW</t>
         </is>
       </c>
     </row>
@@ -1375,12 +1375,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>PANW</t>
+          <t>ALLO</t>
         </is>
       </c>
     </row>
@@ -1390,12 +1390,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>PAYX</t>
+          <t>BCEI</t>
         </is>
       </c>
     </row>
@@ -1405,12 +1405,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PEG</t>
+          <t>BPMC</t>
         </is>
       </c>
     </row>
@@ -1420,12 +1420,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>PEGA</t>
+          <t>BTU</t>
         </is>
       </c>
     </row>
@@ -1435,12 +1435,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>PEP</t>
+          <t>CEIX</t>
         </is>
       </c>
     </row>
@@ -1450,12 +1450,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>PFPT</t>
+          <t>COG</t>
         </is>
       </c>
     </row>
@@ -1465,12 +1465,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>PHR</t>
+          <t>CRC</t>
         </is>
       </c>
     </row>
@@ -1480,12 +1480,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>PMT</t>
+          <t>DO</t>
         </is>
       </c>
     </row>
@@ -1495,12 +1495,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>RJF</t>
+          <t>ENTA</t>
         </is>
       </c>
     </row>
@@ -1510,12 +1510,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>RMD</t>
+          <t>EQT</t>
         </is>
       </c>
     </row>
@@ -1525,12 +1525,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SIBN</t>
+          <t>GTHX</t>
         </is>
       </c>
     </row>
@@ -1540,12 +1540,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SMTC</t>
+          <t>LBRT</t>
         </is>
       </c>
     </row>
@@ -1555,12 +1555,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>PEB</t>
         </is>
       </c>
     </row>
@@ -1570,12 +1570,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>SSD</t>
+          <t>PUMP</t>
         </is>
       </c>
     </row>
@@ -1585,12 +1585,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>STWD</t>
+          <t>PVAC</t>
         </is>
       </c>
     </row>
@@ -1600,12 +1600,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>TCPC</t>
+          <t>RLI</t>
         </is>
       </c>
     </row>
@@ -1615,12 +1615,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>TENB</t>
+          <t>SCHN</t>
         </is>
       </c>
     </row>
@@ -1630,12 +1630,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>TMO</t>
+          <t>SGMO</t>
         </is>
       </c>
     </row>
@@ -1645,12 +1645,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>TRMB</t>
+          <t>UNFI</t>
         </is>
       </c>
     </row>
@@ -1660,12 +1660,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>TROW</t>
+          <t>VIRT</t>
         </is>
       </c>
     </row>
@@ -1675,12 +1675,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>TRU</t>
+          <t>VYGR</t>
         </is>
       </c>
     </row>
@@ -1690,477 +1690,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>TTEK</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>TWO</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>UMH</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>VRTX</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>WDAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>WMS</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>WRB</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>XRAY</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>YMAB</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>ZBH</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>AAWW</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>BCEI</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>BLFS</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>BPMC</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>BTU</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>CEIX</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>CLR</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>COG</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>DFIN</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>DO</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>ENTA</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>108</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>EOLS</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>EQT</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>FIXX</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>111</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>FSLR</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>112</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>GOGO</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>LBRT</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>PDCE</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>115</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>SCHN</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>116</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>SFIX</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>117</v>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>SXC</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>118</v>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>WNC</t>
+          <t>X</t>
         </is>
       </c>
     </row>

</xml_diff>